<commit_message>
Update Wifi bootloader prelim CPD 4.xlsx
</commit_message>
<xml_diff>
--- a/Wifi bootloader prelim CPD 4.xlsx
+++ b/Wifi bootloader prelim CPD 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\WIFI app\WIFI Config App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\Booyco HMI Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5933A00B-CF06-4B33-988E-E105D47D9F6B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AB7F78-325C-474E-A135-CE39F42BC825}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="840" windowWidth="24840" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -737,7 +737,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>